<commit_message>
updated calculation and added some buttons
</commit_message>
<xml_diff>
--- a/RD_test.xlsx
+++ b/RD_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IrisReitsmaRiskQuest\Documents\GitHub\dasbhoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF468A8-50B9-450F-B458-F833317D3F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA4A93C-ABA6-4E20-8B3E-36787D7F8976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9105" windowWidth="29040" windowHeight="15840" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
+    <workbookView xWindow="13245" yWindow="-16455" windowWidth="29040" windowHeight="15840" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -584,10 +584,10 @@
     <t>Company activities are included in EU Green Taxonomy and fully complies to CSRD, but does much more in the field of sustainability (e.g. on social factors). Furthermore, future policies (e.g. EU ecodesign guidelines) will certainly not impact the company</t>
   </si>
   <si>
-    <t>Hybrid (partly fixed, partly performance based)</t>
-  </si>
-  <si>
-    <t>Company is sustainable in current policies and a strong belief that company is ready for future policies</t>
+    <t xml:space="preserve">Company is regarded as sustainable in current policies and a strong belief that company is ready for future policies </t>
+  </si>
+  <si>
+    <t>Hybrid: partly fixed, partly performance based</t>
   </si>
 </sst>
 </file>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC94184-36DC-4334-8EC3-79CE319DCC44}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>126</v>
@@ -1664,9 +1664,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="4:5" ht="48" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:5" ht="36" x14ac:dyDescent="0.3">
       <c r="D66" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>180</v>
@@ -1869,20 +1869,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1905,6 +1905,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1919,12 +1927,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>